<commit_message>
email id details updated
</commit_message>
<xml_diff>
--- a/projectMember_Details.xlsx
+++ b/projectMember_Details.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codehustlers\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEEA613-6904-408B-A375-B7701345AE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>GROUP CODE HUSTLER</t>
   </si>
@@ -94,13 +88,31 @@
   </si>
   <si>
     <t>email_Id</t>
+  </si>
+  <si>
+    <t>sampadakadam98@gmail.com</t>
+  </si>
+  <si>
+    <t>bisenpooja5413@gmail.com</t>
+  </si>
+  <si>
+    <t>kumbharomkar45@gmail.com</t>
+  </si>
+  <si>
+    <t>pritirpatil187@gmail.com</t>
+  </si>
+  <si>
+    <t>mahadikamit086@gmail.com</t>
+  </si>
+  <si>
+    <t>shivanisb234@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +124,14 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -388,10 +408,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -450,8 +471,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="15" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -510,7 +541,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -545,7 +576,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -722,34 +753,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="6.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="4:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="4:11" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="4:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="14" t="s">
         <v>0</v>
       </c>
@@ -761,7 +792,7 @@
       <c r="J3" s="15"/>
       <c r="K3" s="16"/>
     </row>
-    <row r="4" spans="4:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="4:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="17"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
@@ -771,7 +802,7 @@
       <c r="J4" s="18"/>
       <c r="K4" s="19"/>
     </row>
-    <row r="5" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="4:11" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D5" s="11" t="s">
         <v>1</v>
       </c>
@@ -797,7 +828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D6" s="2">
         <v>1</v>
       </c>
@@ -819,9 +850,11 @@
       <c r="J6" s="10">
         <v>0.5</v>
       </c>
-      <c r="K6" s="10"/>
+      <c r="K6" s="21" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D7" s="4">
         <v>2</v>
       </c>
@@ -843,9 +876,11 @@
       <c r="J7" s="6">
         <v>0.7</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="20" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D8" s="4">
         <v>3</v>
       </c>
@@ -867,9 +902,11 @@
       <c r="J8" s="6">
         <v>0.7</v>
       </c>
-      <c r="K8" s="6"/>
+      <c r="K8" s="20" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D9" s="4">
         <v>4</v>
       </c>
@@ -891,9 +928,11 @@
       <c r="J9" s="6">
         <v>0.5</v>
       </c>
-      <c r="K9" s="6"/>
+      <c r="K9" s="20" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="4">
         <v>5</v>
       </c>
@@ -915,9 +954,11 @@
       <c r="J10" s="6">
         <v>0.6</v>
       </c>
-      <c r="K10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="11" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="7">
         <v>6</v>
       </c>
@@ -939,13 +980,22 @@
       <c r="J11" s="9">
         <v>0.7</v>
       </c>
-      <c r="K11" s="9"/>
+      <c r="K11" s="22" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D3:K4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K7" r:id="rId1"/>
+    <hyperlink ref="K9" r:id="rId2"/>
+    <hyperlink ref="K6" r:id="rId3"/>
+    <hyperlink ref="K8" r:id="rId4"/>
+    <hyperlink ref="K11" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>